<commit_message>
CORREÇÃO DO ENCERRAMENTO NO FINAL DA EXECUÇÃO DO EXE
</commit_message>
<xml_diff>
--- a/dados/dados_documentos.xlsx
+++ b/dados/dados_documentos.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\OneDrive\Documentos\AutomatizadorDocumentos\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B987B21-C4AE-458F-891F-CD47986D95F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2180D704-FBFF-4D50-A47A-E54504E32386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>CAMINHO</t>
   </si>
@@ -52,25 +52,7 @@
     <t>modelosPadrao\</t>
   </si>
   <si>
-    <t>ASSINATURA DO CONTRATO_DU</t>
-  </si>
-  <si>
     <t>.docx</t>
-  </si>
-  <si>
-    <t>modelosPadrao\ASSINATURA DO CONTRATO_DU.docx</t>
-  </si>
-  <si>
-    <t>PBH</t>
-  </si>
-  <si>
-    <t>90/2025</t>
-  </si>
-  <si>
-    <t>PE</t>
-  </si>
-  <si>
-    <t>MG</t>
   </si>
 </sst>
 </file>
@@ -434,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +430,7 @@
     <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" bestFit="1" customWidth="1"/>
   </cols>
@@ -486,30 +468,27 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="2">
-        <v>45943</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
+      <c r="D2" t="str">
+        <f>A2&amp;B2&amp;C2</f>
+        <v>modelosPadrao\.docx</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="str">
+        <f>A3&amp;B3&amp;C3</f>
+        <v>modelosPadrao\.docx</v>
+      </c>
+      <c r="G3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>